<commit_message>
Cache-Dateien entfernt und Aufgabenliste aktualisiert
</commit_message>
<xml_diff>
--- a/aufgaben.xlsx
+++ b/aufgaben.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19417E3D-E15E-4933-91C1-0AF16DCD5655}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA32CFC-1DA0-4A9F-9F0F-5597A0290CA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24840" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,9 +141,6 @@
 Welche Ergebnisse werden wann benötigt?</t>
   </si>
   <si>
-    <t>Github-Repo anlegen, Dateistruktur verwalten</t>
-  </si>
-  <si>
     <t>Gemeinsames Repository</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>Klärung, wie Prozess vorher aussah und nachher aussehen soll</t>
+  </si>
+  <si>
+    <t>Github-Repo anlegen, Dateistruktur verwalten, Template für finales Dokument erstellen</t>
   </si>
 </sst>
 </file>
@@ -622,8 +622,8 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,19 +640,19 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
@@ -661,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
       </c>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0</v>
       </c>
@@ -720,10 +720,10 @@
         <v>17</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>29</v>
@@ -744,19 +744,19 @@
         <v>20</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>75</v>
-      </c>
       <c r="E5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" s="6"/>
     </row>
@@ -768,16 +768,16 @@
         <v>24</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="F6" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>33</v>
@@ -795,7 +795,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>29</v>
@@ -816,16 +816,16 @@
         <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>34</v>
@@ -840,16 +840,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>35</v>
@@ -864,16 +864,16 @@
         <v>22</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>36</v>
@@ -888,16 +888,16 @@
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>36</v>
@@ -912,16 +912,16 @@
         <v>25</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>36</v>
@@ -936,16 +936,16 @@
         <v>26</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>36</v>
@@ -960,16 +960,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>36</v>
@@ -984,16 +984,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>36</v>
@@ -1008,16 +1008,16 @@
         <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>36</v>
@@ -1032,16 +1032,16 @@
         <v>11</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>63</v>
-      </c>
       <c r="F17" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>36</v>
@@ -1056,16 +1056,16 @@
         <v>19</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>36</v>
@@ -1080,16 +1080,16 @@
         <v>7</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>36</v>
@@ -1104,16 +1104,16 @@
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>36</v>
@@ -1128,16 +1128,16 @@
         <v>16</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>36</v>
@@ -1152,16 +1152,16 @@
         <v>14</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>36</v>
@@ -1176,16 +1176,16 @@
         <v>21</v>
       </c>
       <c r="C23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>66</v>
-      </c>
       <c r="E23" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>36</v>
@@ -1200,16 +1200,16 @@
         <v>23</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>36</v>

</xml_diff>